<commit_message>
payless anonymous and authenticated
</commit_message>
<xml_diff>
--- a/payless-web-tests/testData/Anonymous.xlsx
+++ b/payless-web-tests/testData/Anonymous.xlsx
@@ -7,15 +7,15 @@
     <workbookView windowWidth="22368" windowHeight="9215" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Anonymous" sheetId="1" r:id="rId1"/>
+    <sheet name="Authenticated" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="77">
   <si>
     <t>TestMethodName</t>
   </si>
@@ -131,10 +131,10 @@
     <t>Thailand</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>M</t>
+    <t>Albert</t>
+  </si>
+  <si>
+    <t>Edsin</t>
   </si>
   <si>
     <t>automation@yopmail.com</t>
@@ -146,6 +146,12 @@
     <t>MUZZ002</t>
   </si>
   <si>
+    <t>06/13/2023</t>
+  </si>
+  <si>
+    <t>06/22/2023</t>
+  </si>
+  <si>
     <t>Paylater</t>
   </si>
   <si>
@@ -159,12 +165,6 @@
   </si>
   <si>
     <t>U S A</t>
-  </si>
-  <si>
-    <t>Albert</t>
-  </si>
-  <si>
-    <t>Edsin</t>
   </si>
   <si>
     <t>GUZZ002</t>
@@ -254,10 +254,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="h:mm\ AM/PM"/>
-    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="h:mm\ AM/PM"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -275,13 +275,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -289,7 +282,67 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -304,7 +357,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -318,22 +371,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -342,32 +379,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -379,9 +395,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -403,27 +418,12 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -434,43 +434,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -482,120 +602,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -603,18 +615,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -643,11 +643,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -685,17 +691,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -728,156 +728,158 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1200,7 +1202,7 @@
   <dimension ref="A1:AG7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A1:AG7"/>
+      <selection activeCell="A7" sqref="A1:AG7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" outlineLevelRow="6"/>
@@ -1368,17 +1370,17 @@
       <c r="S2" t="s">
         <v>41</v>
       </c>
-      <c r="T2" t="s">
-        <v>41</v>
+      <c r="T2" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="U2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="V2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="W2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="X2" t="s">
         <v>41</v>
@@ -1411,27 +1413,24 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:33">
-      <c r="A3" t="s">
-        <v>33</v>
-      </c>
+    <row r="3" spans="2:33">
       <c r="B3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
         <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F3" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="G3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="H3" t="s">
         <v>40</v>
@@ -1439,13 +1438,13 @@
       <c r="I3">
         <v>9838234567</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="3">
         <v>0.458333333333333</v>
       </c>
       <c r="K3" t="s">
         <v>41</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="3">
         <v>0.979166666666667</v>
       </c>
       <c r="M3" t="s">
@@ -1476,7 +1475,7 @@
         <v>52</v>
       </c>
       <c r="V3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="W3" t="s">
         <v>41</v>
@@ -1512,10 +1511,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:33">
-      <c r="A4" t="s">
-        <v>33</v>
-      </c>
+    <row r="4" spans="2:33">
       <c r="B4" t="s">
         <v>53</v>
       </c>
@@ -1529,10 +1525,10 @@
         <v>41</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="G4" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="H4" t="s">
         <v>40</v>
@@ -1540,7 +1536,7 @@
       <c r="I4">
         <v>9838234567</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="3">
         <v>0.458333333333333</v>
       </c>
       <c r="K4" t="s">
@@ -1577,7 +1573,7 @@
         <v>41</v>
       </c>
       <c r="V4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="W4" t="s">
         <v>41</v>
@@ -1613,10 +1609,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:33">
-      <c r="A5" t="s">
-        <v>33</v>
-      </c>
+    <row r="5" spans="2:33">
       <c r="B5" t="s">
         <v>57</v>
       </c>
@@ -1627,13 +1620,13 @@
         <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="H5" t="s">
         <v>40</v>
@@ -1641,19 +1634,19 @@
       <c r="I5">
         <v>9838234567</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="3">
         <v>0.458333333333333</v>
       </c>
       <c r="K5" t="s">
         <v>41</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="3">
         <v>0.979166666666667</v>
       </c>
       <c r="M5">
         <v>123</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5" s="4">
         <v>343000000000000</v>
       </c>
       <c r="O5" t="s">
@@ -1714,10 +1707,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:33">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
+    <row r="6" spans="2:33">
       <c r="B6" t="s">
         <v>62</v>
       </c>
@@ -1728,13 +1718,13 @@
         <v>54</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="G6" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="H6" t="s">
         <v>40</v>
@@ -1742,7 +1732,7 @@
       <c r="I6">
         <v>9838234567</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="3">
         <v>0.458333333333333</v>
       </c>
       <c r="K6" t="s">
@@ -1754,7 +1744,7 @@
       <c r="M6">
         <v>123</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6" s="4">
         <v>348000000000000</v>
       </c>
       <c r="O6" t="s">
@@ -1815,10 +1805,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:33">
-      <c r="A7" t="s">
-        <v>33</v>
-      </c>
+    <row r="7" spans="2:33">
       <c r="B7" t="s">
         <v>63</v>
       </c>
@@ -1829,13 +1816,13 @@
         <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F7" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="G7" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="H7" t="s">
         <v>40</v>
@@ -1843,7 +1830,7 @@
       <c r="I7">
         <v>9838234567</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="3">
         <v>0.458333333333333</v>
       </c>
       <c r="K7" t="s">
@@ -1880,7 +1867,7 @@
         <v>41</v>
       </c>
       <c r="V7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="W7" t="s">
         <v>41</v>
@@ -1928,10 +1915,45 @@
   <dimension ref="A1:AG7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="$A1:$XFD1048576"/>
+      <selection activeCell="A3" sqref="A1:AG7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.6" outlineLevelRow="6"/>
+  <cols>
+    <col min="1" max="1" width="29.5" customWidth="1"/>
+    <col min="2" max="2" width="60.7" customWidth="1"/>
+    <col min="3" max="3" width="9.3" customWidth="1"/>
+    <col min="4" max="4" width="14.7" customWidth="1"/>
+    <col min="5" max="5" width="8.2" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="9.7" customWidth="1"/>
+    <col min="8" max="8" width="6.1" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="11.4" customWidth="1"/>
+    <col min="11" max="11" width="15.8" customWidth="1"/>
+    <col min="12" max="12" width="12.5" customWidth="1"/>
+    <col min="13" max="13" width="4.8" customWidth="1"/>
+    <col min="14" max="14" width="10.6" customWidth="1"/>
+    <col min="15" max="15" width="9.3" customWidth="1"/>
+    <col min="16" max="16" width="8.7" customWidth="1"/>
+    <col min="17" max="17" width="4.6" customWidth="1"/>
+    <col min="18" max="18" width="15.2" customWidth="1"/>
+    <col min="19" max="19" width="17.2" customWidth="1"/>
+    <col min="20" max="20" width="11.3" customWidth="1"/>
+    <col min="21" max="21" width="12.3" customWidth="1"/>
+    <col min="22" max="22" width="16.9" customWidth="1"/>
+    <col min="23" max="23" width="9.3" customWidth="1"/>
+    <col min="24" max="24" width="6" customWidth="1"/>
+    <col min="25" max="25" width="14.5" customWidth="1"/>
+    <col min="26" max="26" width="8.2" customWidth="1"/>
+    <col min="27" max="27" width="4.7" customWidth="1"/>
+    <col min="28" max="28" width="5.8" customWidth="1"/>
+    <col min="29" max="29" width="8.3" customWidth="1"/>
+    <col min="30" max="30" width="12.6" customWidth="1"/>
+    <col min="31" max="31" width="10.4" customWidth="1"/>
+    <col min="32" max="32" width="18.2" customWidth="1"/>
+    <col min="33" max="33" width="17.7" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:33">
       <c r="A1" t="s">
@@ -2045,7 +2067,7 @@
         <v>67</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
         <v>41</v>
@@ -2062,13 +2084,13 @@
       <c r="I2" t="s">
         <v>41</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="3">
         <v>0.458333333333333</v>
       </c>
       <c r="K2" t="s">
         <v>41</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="3">
         <v>0.979166666666667</v>
       </c>
       <c r="M2" t="s">
@@ -2099,7 +2121,7 @@
         <v>52</v>
       </c>
       <c r="V2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="W2" t="s">
         <v>41</v>
@@ -2136,9 +2158,7 @@
       </c>
     </row>
     <row r="3" spans="1:33">
-      <c r="A3" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="A3" s="2"/>
       <c r="B3" t="s">
         <v>70</v>
       </c>
@@ -2163,7 +2183,7 @@
       <c r="I3" t="s">
         <v>41</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="3">
         <v>0.458333333333333</v>
       </c>
       <c r="K3" t="s">
@@ -2200,7 +2220,7 @@
         <v>41</v>
       </c>
       <c r="V3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="W3" t="s">
         <v>41</v>
@@ -2237,9 +2257,7 @@
       </c>
     </row>
     <row r="4" spans="1:33">
-      <c r="A4" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="A4" s="2"/>
       <c r="B4" t="s">
         <v>71</v>
       </c>
@@ -2301,10 +2319,10 @@
         <v>41</v>
       </c>
       <c r="V4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="W4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="X4" t="s">
         <v>41</v>
@@ -2338,9 +2356,7 @@
       </c>
     </row>
     <row r="5" spans="1:33">
-      <c r="A5" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="A5" s="2"/>
       <c r="B5" t="s">
         <v>72</v>
       </c>
@@ -2348,7 +2364,7 @@
         <v>67</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
         <v>41</v>
@@ -2365,13 +2381,13 @@
       <c r="I5" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="3">
         <v>0.458333333333333</v>
       </c>
       <c r="K5" t="s">
         <v>41</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="3">
         <v>0.979166666666667</v>
       </c>
       <c r="M5">
@@ -2439,9 +2455,7 @@
       </c>
     </row>
     <row r="6" spans="1:33">
-      <c r="A6" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="A6" s="2"/>
       <c r="B6" t="s">
         <v>75</v>
       </c>
@@ -2466,7 +2480,7 @@
       <c r="I6" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="3">
         <v>0.458333333333333</v>
       </c>
       <c r="K6" t="s">
@@ -2540,9 +2554,7 @@
       </c>
     </row>
     <row r="7" spans="1:33">
-      <c r="A7" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="A7" s="2"/>
       <c r="B7" t="s">
         <v>76</v>
       </c>
@@ -2567,13 +2579,13 @@
       <c r="I7" t="s">
         <v>41</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="3">
         <v>0.458333333333333</v>
       </c>
       <c r="K7" t="s">
         <v>41</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="3">
         <v>0.979166666666667</v>
       </c>
       <c r="M7">

</xml_diff>

<commit_message>
updated budget test cases
</commit_message>
<xml_diff>
--- a/payless-web-tests/testData/Anonymous.xlsx
+++ b/payless-web-tests/testData/Anonymous.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10212"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/StatusNeo/Downloads/web_framework_updated branch 16 march/ecom-us-web/payless-web-tests/testData/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3875F8DB-3FF9-0C4F-B9FD-9125E6FAEDF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9215" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Anonymous" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="106">
   <si>
     <t>TestMethodName</t>
   </si>
@@ -331,20 +337,16 @@
   </si>
   <si>
     <t>Payless@123</t>
+  </si>
+  <si>
+    <t>Testuser12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="h:mm\ AM/PM"/>
-  </numFmts>
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -356,355 +358,40 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Courier New"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -712,334 +399,46 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="18" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1297,31 +696,31 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP11"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="AO21" sqref="AO21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.1111111111111" customWidth="1"/>
-    <col min="2" max="2" width="74.2222222222222" customWidth="1"/>
-    <col min="9" max="9" width="13.1111111111111"/>
-    <col min="33" max="33" width="19.8888888888889" customWidth="1"/>
-    <col min="34" max="34" width="11.7777777777778" customWidth="1"/>
-    <col min="35" max="35" width="10.1111111111111" customWidth="1"/>
-    <col min="37" max="37" width="66.5555555555556" customWidth="1"/>
-    <col min="38" max="38" width="18.7777777777778" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" customWidth="1"/>
+    <col min="2" max="2" width="74.1640625" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625"/>
+    <col min="33" max="33" width="19.83203125" customWidth="1"/>
+    <col min="34" max="34" width="11.83203125" customWidth="1"/>
+    <col min="35" max="35" width="10.1640625" customWidth="1"/>
+    <col min="37" max="37" width="66.5" customWidth="1"/>
+    <col min="38" max="38" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" spans="1:42">
+    <row r="1" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1449,7 +848,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" ht="15.6" spans="1:37">
+    <row r="2" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1507,7 +906,7 @@
       <c r="S2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="T2" s="1" t="s">
         <v>51</v>
       </c>
       <c r="U2" s="1" t="s">
@@ -1558,11 +957,11 @@
       <c r="AJ2" t="s">
         <v>49</v>
       </c>
-      <c r="AK2" s="10" t="s">
+      <c r="AK2" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" ht="15.6" spans="1:37">
+    <row r="3" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -1590,13 +989,13 @@
       <c r="I3" s="1">
         <v>9838234567</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>49</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>49</v>
       </c>
       <c r="M3" s="1" t="s">
@@ -1620,7 +1019,7 @@
       <c r="S3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="T3" s="7" t="s">
+      <c r="T3" s="1" t="s">
         <v>51</v>
       </c>
       <c r="U3" s="1" t="s">
@@ -1671,11 +1070,11 @@
       <c r="AJ3" t="s">
         <v>49</v>
       </c>
-      <c r="AK3" s="10" t="s">
+      <c r="AK3" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" ht="15.6" spans="1:37">
+    <row r="4" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -1703,8 +1102,8 @@
       <c r="I4" s="1">
         <v>9838234567</v>
       </c>
-      <c r="J4" s="6">
-        <v>0.458333333333333</v>
+      <c r="J4" s="5">
+        <v>0.45833333333333298</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>49</v>
@@ -1784,11 +1183,11 @@
       <c r="AJ4" t="s">
         <v>49</v>
       </c>
-      <c r="AK4" s="10" t="s">
+      <c r="AK4" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" ht="15.6" spans="1:37">
+    <row r="5" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -1816,19 +1215,19 @@
       <c r="I5" s="1">
         <v>9838234567</v>
       </c>
-      <c r="J5" s="6">
-        <v>0.458333333333333</v>
+      <c r="J5" s="5">
+        <v>0.45833333333333298</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L5" s="6">
-        <v>0.979166666666667</v>
+      <c r="L5" s="5">
+        <v>0.97916666666666696</v>
       </c>
       <c r="M5" s="1">
         <v>123</v>
       </c>
-      <c r="N5" s="9">
+      <c r="N5" s="6">
         <v>343000000000000</v>
       </c>
       <c r="O5" s="1" t="s">
@@ -1897,11 +1296,11 @@
       <c r="AJ5" t="s">
         <v>49</v>
       </c>
-      <c r="AK5" s="10" t="s">
+      <c r="AK5" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" ht="15.6" spans="1:37">
+    <row r="6" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -1929,8 +1328,8 @@
       <c r="I6" s="1">
         <v>9838234567</v>
       </c>
-      <c r="J6" s="6">
-        <v>0.458333333333333</v>
+      <c r="J6" s="5">
+        <v>0.45833333333333298</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>49</v>
@@ -1941,7 +1340,7 @@
       <c r="M6" s="1">
         <v>123</v>
       </c>
-      <c r="N6" s="9">
+      <c r="N6" s="6">
         <v>348000000000000</v>
       </c>
       <c r="O6" s="1" t="s">
@@ -2010,11 +1409,11 @@
       <c r="AJ6" t="s">
         <v>49</v>
       </c>
-      <c r="AK6" s="10" t="s">
+      <c r="AK6" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7" ht="15.6" spans="1:37">
+    <row r="7" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -2042,8 +1441,8 @@
       <c r="I7" s="1">
         <v>9838234567</v>
       </c>
-      <c r="J7" s="6">
-        <v>0.458333333333333</v>
+      <c r="J7" s="5">
+        <v>0.45833333333333298</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>49</v>
@@ -2123,11 +1522,11 @@
       <c r="AJ7" t="s">
         <v>49</v>
       </c>
-      <c r="AK7" s="10" t="s">
+      <c r="AK7" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" ht="15.6" spans="1:37">
+    <row r="8" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -2236,11 +1635,11 @@
       <c r="AJ8" t="s">
         <v>49</v>
       </c>
-      <c r="AK8" s="10" t="s">
+      <c r="AK8" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" ht="15.6" spans="1:37">
+    <row r="9" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -2298,7 +1697,7 @@
       <c r="S9" t="s">
         <v>49</v>
       </c>
-      <c r="T9" s="7" t="s">
+      <c r="T9" s="1" t="s">
         <v>51</v>
       </c>
       <c r="U9" s="1" t="s">
@@ -2349,11 +1748,11 @@
       <c r="AJ9" t="s">
         <v>63</v>
       </c>
-      <c r="AK9" s="10" t="s">
+      <c r="AK9" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" ht="15.6" spans="1:37">
+    <row r="10" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -2381,13 +1780,13 @@
       <c r="I10" s="1">
         <v>9838234567</v>
       </c>
-      <c r="J10" s="6" t="s">
+      <c r="J10" s="5" t="s">
         <v>49</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L10" s="6" t="s">
+      <c r="L10" s="5" t="s">
         <v>49</v>
       </c>
       <c r="M10" s="1" t="s">
@@ -2411,7 +1810,7 @@
       <c r="S10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="T10" s="7" t="s">
+      <c r="T10" s="1" t="s">
         <v>51</v>
       </c>
       <c r="U10" s="1" t="s">
@@ -2462,38 +1861,36 @@
       <c r="AJ10" t="s">
         <v>49</v>
       </c>
-      <c r="AK10" s="10" t="s">
+      <c r="AK10" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" ht="15.6" spans="3:3">
+    <row r="11" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="C11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AP11"/>
   <sheetViews>
-    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="AP1" sqref="AP1"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="S2" sqref="A1:AP10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.1111111111111" customWidth="1"/>
-    <col min="2" max="2" width="68.1111111111111" customWidth="1"/>
-    <col min="33" max="33" width="19.8888888888889" customWidth="1"/>
-    <col min="37" max="37" width="66.5555555555556" customWidth="1"/>
-    <col min="38" max="38" width="18.7777777777778" customWidth="1"/>
+    <col min="1" max="1" width="33.1640625" customWidth="1"/>
+    <col min="2" max="2" width="68.1640625" customWidth="1"/>
+    <col min="33" max="33" width="19.83203125" customWidth="1"/>
+    <col min="37" max="37" width="66.5" customWidth="1"/>
+    <col min="38" max="38" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" spans="1:42">
+    <row r="1" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2621,8 +2018,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" ht="15.6" spans="1:37">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:42" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2649,13 +2046,13 @@
       <c r="I2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>49</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="5" t="s">
         <v>49</v>
       </c>
       <c r="M2" s="1" t="s">
@@ -2673,8 +2070,8 @@
       <c r="Q2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="R2" s="1" t="s">
-        <v>79</v>
+      <c r="R2" s="8" t="s">
+        <v>105</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>80</v>
@@ -2730,14 +2127,12 @@
       <c r="AJ2" t="s">
         <v>49</v>
       </c>
-      <c r="AK2" s="8" t="s">
+      <c r="AK2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" ht="15.6" spans="1:37">
-      <c r="A3" s="4" t="s">
-        <v>76</v>
-      </c>
+    <row r="3" spans="1:42" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
         <v>83</v>
       </c>
@@ -2762,8 +2157,8 @@
       <c r="I3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J3" s="6">
-        <v>0.458333333333333</v>
+      <c r="J3" s="5">
+        <v>0.45833333333333298</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>49</v>
@@ -2843,14 +2238,12 @@
       <c r="AJ3" t="s">
         <v>49</v>
       </c>
-      <c r="AK3" s="8" t="s">
+      <c r="AK3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" ht="15.6" spans="1:37">
-      <c r="A4" s="4" t="s">
-        <v>76</v>
-      </c>
+    <row r="4" spans="1:42" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
       <c r="B4" s="1" t="s">
         <v>84</v>
       </c>
@@ -2956,14 +2349,12 @@
       <c r="AJ4" t="s">
         <v>49</v>
       </c>
-      <c r="AK4" s="8" t="s">
+      <c r="AK4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" ht="15.6" spans="1:37">
-      <c r="A5" s="4" t="s">
-        <v>76</v>
-      </c>
+    <row r="5" spans="1:42" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
       <c r="B5" s="1" t="s">
         <v>85</v>
       </c>
@@ -2988,14 +2379,14 @@
       <c r="I5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J5" s="6">
-        <v>0.458333333333333</v>
+      <c r="J5" s="5">
+        <v>0.45833333333333298</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L5" s="6">
-        <v>0.979166666666667</v>
+      <c r="L5" s="5">
+        <v>0.97916666666666696</v>
       </c>
       <c r="M5" s="1">
         <v>123</v>
@@ -3069,14 +2460,12 @@
       <c r="AJ5" t="s">
         <v>49</v>
       </c>
-      <c r="AK5" s="8" t="s">
+      <c r="AK5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" ht="15.6" spans="1:37">
-      <c r="A6" s="4" t="s">
-        <v>76</v>
-      </c>
+    <row r="6" spans="1:42" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
       <c r="B6" s="1" t="s">
         <v>88</v>
       </c>
@@ -3101,8 +2490,8 @@
       <c r="I6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="6">
-        <v>0.458333333333333</v>
+      <c r="J6" s="5">
+        <v>0.45833333333333298</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>49</v>
@@ -3182,14 +2571,12 @@
       <c r="AJ6" t="s">
         <v>49</v>
       </c>
-      <c r="AK6" s="8" t="s">
+      <c r="AK6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7" ht="15.6" spans="1:37">
-      <c r="A7" s="4" t="s">
-        <v>76</v>
-      </c>
+    <row r="7" spans="1:42" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
       <c r="B7" s="1" t="s">
         <v>89</v>
       </c>
@@ -3214,14 +2601,14 @@
       <c r="I7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J7" s="6">
-        <v>0.458333333333333</v>
+      <c r="J7" s="5">
+        <v>0.45833333333333298</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L7" s="6">
-        <v>0.979166666666667</v>
+      <c r="L7" s="5">
+        <v>0.97916666666666696</v>
       </c>
       <c r="M7" s="1">
         <v>123</v>
@@ -3295,14 +2682,12 @@
       <c r="AJ7" t="s">
         <v>49</v>
       </c>
-      <c r="AK7" s="8" t="s">
+      <c r="AK7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" ht="15.6" spans="1:37">
-      <c r="A8" s="4" t="s">
-        <v>76</v>
-      </c>
+    <row r="8" spans="1:42" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
       <c r="B8" t="s">
         <v>90</v>
       </c>
@@ -3357,7 +2742,7 @@
       <c r="S8" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="T8" s="7" t="s">
+      <c r="T8" s="1" t="s">
         <v>51</v>
       </c>
       <c r="U8" s="1" t="s">
@@ -3408,14 +2793,12 @@
       <c r="AJ8" t="s">
         <v>49</v>
       </c>
-      <c r="AK8" s="8" t="s">
+      <c r="AK8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" ht="15.6" spans="1:37">
-      <c r="A9" s="4" t="s">
-        <v>76</v>
-      </c>
+    <row r="9" spans="1:42" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
       <c r="B9" t="s">
         <v>93</v>
       </c>
@@ -3470,7 +2853,7 @@
       <c r="S9" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="T9" s="7" t="s">
+      <c r="T9" s="1" t="s">
         <v>51</v>
       </c>
       <c r="U9" s="1" t="s">
@@ -3521,14 +2904,12 @@
       <c r="AJ9" t="s">
         <v>63</v>
       </c>
-      <c r="AK9" s="8" t="s">
+      <c r="AK9" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" ht="15.6" spans="1:37">
-      <c r="A10" s="4" t="s">
-        <v>76</v>
-      </c>
+    <row r="10" spans="1:42" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
       <c r="B10" t="s">
         <v>94</v>
       </c>
@@ -3583,7 +2964,7 @@
       <c r="S10" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="T10" s="7" t="s">
+      <c r="T10" s="1" t="s">
         <v>49</v>
       </c>
       <c r="U10" s="1" t="s">
@@ -3634,37 +3015,35 @@
       <c r="AJ10" t="s">
         <v>49</v>
       </c>
-      <c r="AK10" s="8" t="s">
+      <c r="AK10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="5"/>
+    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AP3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.4444444444444" customWidth="1"/>
-    <col min="2" max="2" width="39.2222222222222" customWidth="1"/>
-    <col min="38" max="38" width="18.7777777777778" customWidth="1"/>
-    <col min="42" max="42" width="11.5555555555556" customWidth="1"/>
+    <col min="1" max="1" width="29.5" customWidth="1"/>
+    <col min="2" max="2" width="39.1640625" customWidth="1"/>
+    <col min="38" max="38" width="18.83203125" customWidth="1"/>
+    <col min="42" max="42" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.6" spans="1:42">
+    <row r="1" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3792,7 +3171,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" ht="15.6" spans="1:42">
+    <row r="2" spans="1:42" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>96</v>
       </c>
@@ -3920,14 +3299,13 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AP2" r:id="rId1" display="Payless@123"/>
+    <hyperlink ref="AP2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>